<commit_message>
finished to order list
</commit_message>
<xml_diff>
--- a/sedani/estop/estop-1.3-inventory.xlsx
+++ b/sedani/estop/estop-1.3-inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78A7EC9-8B73-4885-93A0-8F942D91D3E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6C1A30-A7AB-46A6-9CB6-973435FCEB28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>296-39452-1-ND</t>
   </si>
@@ -322,6 +322,15 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>200mA hold, 400mA trip</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Needed per board</t>
   </si>
 </sst>
 </file>
@@ -683,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -695,7 +704,7 @@
     <col min="4" max="4" width="8.88671875" style="1"/>
     <col min="5" max="5" width="18.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.21875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="8" customWidth="1"/>
     <col min="8" max="8" width="8.88671875" style="1"/>
     <col min="9" max="9" width="21.88671875" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.21875" style="1" customWidth="1"/>
@@ -725,7 +734,9 @@
       <c r="F1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="1"/>
+      <c r="G1" s="8" t="s">
+        <v>99</v>
+      </c>
       <c r="I1" s="1" t="s">
         <v>18</v>
       </c>
@@ -733,7 +744,7 @@
         <v>22</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -796,6 +807,9 @@
         <f t="shared" ref="F3:F25" si="0">IF(D3&gt;E3, D3-E3, 0)</f>
         <v>1</v>
       </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
       <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
@@ -831,6 +845,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="G4" s="8">
+        <v>3</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
@@ -865,6 +882,9 @@
       <c r="F5" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="G5" s="8">
+        <v>3</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>23</v>
@@ -935,6 +955,9 @@
       <c r="F7" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
+      </c>
+      <c r="G7" s="8">
+        <v>15</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>49</v>
@@ -1276,6 +1299,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="G17" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
@@ -1295,7 +1321,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="8">
+        <v>5</v>
+      </c>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1339,9 +1367,12 @@
         <v>2</v>
       </c>
       <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2"/>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G20" s="8">
+        <v>6</v>
+      </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
@@ -1363,9 +1394,12 @@
         <v>2</v>
       </c>
       <c r="F21" s="8">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G21" s="8">
+        <v>3</v>
+      </c>
       <c r="M21" s="2"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
@@ -1386,7 +1420,11 @@
         <v>2</v>
       </c>
       <c r="F22" s="8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G22" s="8">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
@@ -1410,6 +1448,9 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="G23" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1432,8 +1473,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G24" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -1448,11 +1492,14 @@
         <v>3</v>
       </c>
       <c r="E25" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>